<commit_message>
Added second reporting (DTOE table) extract activities to previous Process Workflow and verified report delivery to network share
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sv_rpabot24\Documents\UiPath\TIOS_DTOE_Tableau_Dispatcher-main\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sv_rpabot24\Documents\UiPath\TIOS_DTOE_Tableau_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1CB652-1E3B-4812-91C7-CBF946323CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956CB0A2-E2D5-4023-B315-0E5DBD58643B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29925" yWindow="1125" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30270" yWindow="1470" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Changes made to process
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sv_rpabot24\Documents\UiPath\TIOS_DTOE_Tableau_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956CB0A2-E2D5-4023-B315-0E5DBD58643B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBC660F-D365-4EFE-897F-A6DCEFF7AC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30270" yWindow="1470" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -178,7 +178,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -200,12 +200,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFF8F9FA"/>
-      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
     <font>
@@ -239,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -250,11 +244,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -621,7 +614,7 @@
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -650,10 +643,10 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2827,7 +2820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2876,26 +2869,26 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Root folder changed to permanently reflect FPPS/DTOE in the Config file Initial release (publication) in DEV environment
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sv_rpabot24\Documents\UiPath\TIOS_DTOE_Tableau_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBC660F-D365-4EFE-897F-A6DCEFF7AC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AB90DD-D086-48EB-9E17-9BA5145C7AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>DTOE_Tableau_SuccessURL</t>
+  </si>
+  <si>
+    <t>FPPS/DTOE</t>
   </si>
 </sst>
 </file>
@@ -565,7 +568,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -625,7 +628,9 @@
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Edits made to source file for DataTable2 (UseCase2) Adjustments made to activities
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sv_rpabot24\Documents\UiPath\TIOS_DTOE_Tableau_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AB90DD-D086-48EB-9E17-9BA5145C7AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946FEDA5-5484-4434-98F1-9FFAFBC87C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5850" yWindow="1200" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -567,7 +567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2825,8 +2825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2880,6 +2880,9 @@
       <c r="B2" s="5" t="s">
         <v>44</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="6" t="s">
@@ -2888,6 +2891,9 @@
       <c r="B3" s="6" t="s">
         <v>46</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="7" t="s">
@@ -2896,8 +2902,13 @@
       <c r="B4" s="7" t="s">
         <v>48</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="C5" s="2"/>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>